<commit_message>
rill-analysis: After 0.1.0// Add feature: HtmlExporter and JdbcDataRetriever// Enhance.
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/jdbcDataRetriever_table.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/jdbcDataRetriever_table.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -130,10 +130,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>访问量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>jdbc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -190,14 +186,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>日访问量趋势图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>访问量数据表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>环比差</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -252,6 +240,22 @@
   </si>
   <si>
     <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务器维度日访问量趋势图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日访问量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务器维度日访问量数据表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>downloadFileName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -738,14 +742,14 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1199,11 +1203,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="70059904"/>
-        <c:axId val="70061440"/>
+        <c:axId val="75015296"/>
+        <c:axId val="75016832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70059904"/>
+        <c:axId val="75015296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1212,14 +1216,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70061440"/>
+        <c:crossAx val="75016832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70061440"/>
+        <c:axId val="75016832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +1232,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70059904"/>
+        <c:crossAx val="75015296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1246,7 +1250,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001033" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001033" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001044" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001044" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1324,16 +1328,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="paramTable" displayName="paramTable" ref="A8:G9" insertRow="1" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="paramTable" displayName="paramTable" ref="A8:G9" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="A8:G9"/>
   <tableColumns count="7">
     <tableColumn id="1" name="参数" dataDxfId="6"/>
     <tableColumn id="2" name="名称" dataDxfId="5"/>
-    <tableColumn id="3" name="值" dataDxfId="4"/>
+    <tableColumn id="3" name="值" dataDxfId="4">
+      <calculatedColumnFormula>trend!$B24</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="4" name="类型" dataDxfId="3"/>
-    <tableColumn id="5" name="依赖关系" dataDxfId="2">
-      <calculatedColumnFormula>$B8</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="5" name="依赖关系" dataDxfId="2"/>
     <tableColumn id="6" name="源" dataDxfId="1"/>
     <tableColumn id="7" name="格式" dataDxfId="0"/>
   </tableColumns>
@@ -1651,10 +1655,10 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="2:5">
-      <c r="B2" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="35"/>
+      <c r="B2" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="37"/>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="2:5">
@@ -1662,7 +1666,7 @@
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="25" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -1724,10 +1728,10 @@
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B24" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="35"/>
+      <c r="B24" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="37"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:13" ht="3.75" customHeight="1"/>
@@ -1747,40 +1751,40 @@
     </row>
     <row r="27" spans="1:13" ht="35.25" customHeight="1">
       <c r="B27" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="35" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="I27" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="K27" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H27" s="34" t="s">
+      <c r="L27" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="I27" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="32" t="s">
+      <c r="M27" s="33" t="s">
         <v>47</v>
-      </c>
-      <c r="K27" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="L27" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="M27" s="33" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="16.5" customHeight="1">
@@ -1876,11 +1880,11 @@
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="6.875" customWidth="1"/>
+    <col min="2" max="2" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.875" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1889,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1897,7 +1901,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1905,7 +1909,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1921,7 +1925,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1949,8 +1953,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="4" t="str">
+        <f>trend!$B24</f>
+        <v>服务器维度日访问量数据表</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="12"/>
       <c r="F9" s="11"/>
@@ -1991,20 +2000,20 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="14.25" thickBot="1">
       <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="14.25" thickBot="1">
       <c r="A3" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3">
         <v>47952</v>
@@ -2012,37 +2021,37 @@
     </row>
     <row r="11" spans="1:13">
       <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="J11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" t="s">
         <v>28</v>
       </c>
-      <c r="H11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>29</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>30</v>
-      </c>
-      <c r="M11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -2498,20 +2507,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" thickBot="1">
       <c r="A3" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3">
         <v>45583</v>
@@ -2550,20 +2559,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" thickBot="1">
       <c r="A3" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3">
         <v>136</v>

</xml_diff>